<commit_message>
Merging Josh's heatmap changes, Tim Documentation changes
Merging changes Josh made to heatMap and also documentation changes.
</commit_message>
<xml_diff>
--- a/Documentation/ScheduledTasks.xlsx
+++ b/Documentation/ScheduledTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\OneDrive\Flinders\IT Project\COMP3782Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="11_B8FAB47D3BCFFCB86BD6A932BC3E1AB1A67A14FA" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{CD7BEE58-19D8-413E-9E55-C9F8F9763A83}"/>
+  <xr:revisionPtr revIDLastSave="64" documentId="11_B8FAB47D3BCFFCB86BD6A932BC3E1AB1A67A14FA" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{3F120693-4C1A-411C-80C7-FAD3775AE42B}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="40">
   <si>
     <t>Task ID</t>
   </si>
@@ -125,6 +125,21 @@
   </si>
   <si>
     <t>Work on Widows Implementation</t>
+  </si>
+  <si>
+    <t>Work on Documenation, Complete BSL induction</t>
+  </si>
+  <si>
+    <t>Work on Java implementation, Complete BSL induction</t>
+  </si>
+  <si>
+    <t>Work on LED implementation, Complete BSL induction</t>
+  </si>
+  <si>
+    <t>Work on Raspberry Pi interface, Complete BSL induction</t>
+  </si>
+  <si>
+    <t>Work on brain diagram, Complete BSL induction</t>
   </si>
 </sst>
 </file>
@@ -254,7 +269,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E29">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task Name"/>
@@ -565,8 +580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:E24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -914,6 +929,9 @@
       <c r="D20" s="7">
         <v>43342</v>
       </c>
+      <c r="E20" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" customHeight="1">
       <c r="A21">
@@ -928,6 +946,9 @@
       <c r="D21" s="7">
         <v>43342</v>
       </c>
+      <c r="E21" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" customHeight="1">
       <c r="A22">
@@ -942,6 +963,9 @@
       <c r="D22" s="7">
         <v>43342</v>
       </c>
+      <c r="E22" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" customHeight="1">
       <c r="A23">
@@ -956,6 +980,9 @@
       <c r="D23" s="7">
         <v>43342</v>
       </c>
+      <c r="E23" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" customHeight="1">
       <c r="A24">
@@ -970,12 +997,80 @@
       <c r="D24" s="7">
         <v>43342</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="26" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="27" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="28" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="29" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="E24" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="7">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" s="7">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>37</v>
+      </c>
+      <c r="C27" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="7">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>38</v>
+      </c>
+      <c r="C28" t="s">
+        <v>13</v>
+      </c>
+      <c r="D28" s="7">
+        <v>43349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>39</v>
+      </c>
+      <c r="C29" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="7">
+        <v>43349</v>
+      </c>
+    </row>
     <row r="30" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="31" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="32" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Added Meeting minutes and updated Issues List and Scheduled Task
</commit_message>
<xml_diff>
--- a/Documentation/ScheduledTasks.xlsx
+++ b/Documentation/ScheduledTasks.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\OneDrive\Flinders\IT Project\COMP3782Hardware\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\OneDrive\Flinders\IT Project\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_B8FAB47D3BCFFCB86BD6A932BC3E1AB1A67A14FA" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{24CE8A36-AB50-4E7C-824F-D4757460C79D}"/>
+  <xr:revisionPtr revIDLastSave="121" documentId="11_B8FAB47D3BCFFCB86BD6A932BC3E1AB1A67A14FA" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{CDB45D31-1AF0-4B6A-86E1-7AE5F4CCE9EA}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="50">
   <si>
     <t>Task ID</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t>Work on integrating LED drivers with Raspberry PI</t>
+  </si>
+  <si>
+    <t>Programming Java implementation</t>
+  </si>
+  <si>
+    <t>Continue work on Poster for presentation</t>
   </si>
 </sst>
 </file>
@@ -293,7 +299,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E44">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task Name"/>
@@ -604,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1208,6 +1214,9 @@
       <c r="D35" s="7">
         <v>43363</v>
       </c>
+      <c r="E35" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="36" spans="1:5" ht="15.75" customHeight="1">
       <c r="A36">
@@ -1222,6 +1231,9 @@
       <c r="D36" s="7">
         <v>43363</v>
       </c>
+      <c r="E36" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="37" spans="1:5" ht="15.75" customHeight="1">
       <c r="A37">
@@ -1236,6 +1248,9 @@
       <c r="D37" s="7">
         <v>43363</v>
       </c>
+      <c r="E37" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="38" spans="1:5" ht="15.75" customHeight="1">
       <c r="A38">
@@ -1250,6 +1265,9 @@
       <c r="D38" s="7">
         <v>43363</v>
       </c>
+      <c r="E38" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1">
       <c r="A39">
@@ -1264,12 +1282,80 @@
       <c r="D39" s="7">
         <v>43363</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="41" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="42" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="43" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="44" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="E39" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40" s="7">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>41</v>
+      </c>
+      <c r="C41" t="s">
+        <v>6</v>
+      </c>
+      <c r="D41" s="7">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>49</v>
+      </c>
+      <c r="C42" t="s">
+        <v>15</v>
+      </c>
+      <c r="D42" s="7">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>46</v>
+      </c>
+      <c r="C43" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="7">
+        <v>43370</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>47</v>
+      </c>
+      <c r="C44" t="s">
+        <v>13</v>
+      </c>
+      <c r="D44" s="7">
+        <v>43370</v>
+      </c>
+    </row>
     <row r="45" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="46" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="47" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Updating Shceduled tasks and project
</commit_message>
<xml_diff>
--- a/Documentation/ScheduledTasks.xlsx
+++ b/Documentation/ScheduledTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\OneDrive\Flinders\IT Project\COMP3782Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="22" documentId="102_{D5FC7089-860C-4024-8090-753591C48F14}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{002CAE6A-C110-477A-9ABF-153B74B1EA3D}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="102_{D5FC7089-860C-4024-8090-753591C48F14}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{750828F6-E4CE-4670-B349-5D9B1D54203F}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="A40" sqref="A40:E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Adding Josh's changes to the GiT Repo
</commit_message>
<xml_diff>
--- a/Documentation/ScheduledTasks.xlsx
+++ b/Documentation/ScheduledTasks.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\timot\OneDrive\Flinders\IT Project\COMP3782Hardware\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="24" documentId="102_{D5FC7089-860C-4024-8090-753591C48F14}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{750828F6-E4CE-4670-B349-5D9B1D54203F}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="102_{D5FC7089-860C-4024-8090-753591C48F14}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{B524EBAD-D197-43E2-8D17-046AF6FDAE48}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4470" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="63">
   <si>
     <t>Task ID</t>
   </si>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>Pull usefull data from Raspberry Pi</t>
+  </si>
+  <si>
+    <t>Finish up the poster</t>
+  </si>
+  <si>
+    <t>Demonstrate LED driver on Human Brain</t>
+  </si>
+  <si>
+    <t>Work on Final report and any outstanding documentation</t>
+  </si>
+  <si>
+    <t>Work on LED driver on Raspberry pi</t>
+  </si>
+  <si>
+    <t>Implement Josh's software onto the Raspberry Pi</t>
   </si>
 </sst>
 </file>
@@ -360,7 +375,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E54">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:E59">
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Task ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Task Name"/>
@@ -672,7 +687,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:E49"/>
+      <selection activeCell="A55" sqref="A55:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1530,6 +1545,9 @@
       <c r="D50" s="7">
         <v>43377</v>
       </c>
+      <c r="E50" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="51" spans="1:5" ht="15.75" customHeight="1">
       <c r="A51">
@@ -1544,6 +1562,9 @@
       <c r="D51" s="7">
         <v>43377</v>
       </c>
+      <c r="E51" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="52" spans="1:5" ht="15.75" customHeight="1">
       <c r="A52">
@@ -1558,6 +1579,9 @@
       <c r="D52" s="7">
         <v>43377</v>
       </c>
+      <c r="E52" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="53" spans="1:5" ht="15.75" customHeight="1">
       <c r="A53">
@@ -1572,6 +1596,9 @@
       <c r="D53" s="7">
         <v>43377</v>
       </c>
+      <c r="E53" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="54" spans="1:5" ht="15.75" customHeight="1">
       <c r="A54">
@@ -1586,12 +1613,80 @@
       <c r="D54" s="7">
         <v>43377</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="56" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="57" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="58" spans="1:5" ht="15.75" customHeight="1"/>
-    <row r="59" spans="1:5" ht="15.75" customHeight="1"/>
+      <c r="E54" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>58</v>
+      </c>
+      <c r="C55" t="s">
+        <v>15</v>
+      </c>
+      <c r="D55" s="7">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>59</v>
+      </c>
+      <c r="C56" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56" s="7">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>61</v>
+      </c>
+      <c r="C57" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="7">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>62</v>
+      </c>
+      <c r="C58" t="s">
+        <v>13</v>
+      </c>
+      <c r="D58" s="7">
+        <v>43384</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="15.75" customHeight="1">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>60</v>
+      </c>
+      <c r="C59" t="s">
+        <v>6</v>
+      </c>
+      <c r="D59" s="7">
+        <v>43384</v>
+      </c>
+    </row>
     <row r="60" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="61" spans="1:5" ht="15.75" customHeight="1"/>
     <row r="62" spans="1:5" ht="15.75" customHeight="1"/>

</xml_diff>